<commit_message>
update tuyển dụng recruitmentController.cs,Input.cshtml
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/TuyenDung/UploadContainer/temp.xlsx
+++ b/QUANGHANH2/excel/TCLD/TuyenDung/UploadContainer/temp.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>DANH SÁCH TIẾP NHẬN VÀ BỐ TRÍ CÔNG TÁC ĐỐI VỚI CÔNG NHÂN</t>
     <phoneticPr fontId="1"/>
@@ -95,36 +95,15 @@
     <t>4.867.000</t>
   </si>
   <si>
-    <t>Hoàng Văn Hà</t>
-  </si>
-  <si>
-    <t>TCN</t>
-  </si>
-  <si>
-    <t>Trại Ba,Hồng Kỳ,Yên Thế,Bắc Giang</t>
-  </si>
-  <si>
-    <t>5.305.000</t>
-  </si>
-  <si>
     <t>3/6</t>
   </si>
   <si>
-    <t>4/6</t>
-  </si>
-  <si>
     <t>TKV 01.NI.VII</t>
   </si>
   <si>
     <t>khai thác hầm lò</t>
   </si>
   <si>
-    <t>DL3</t>
-  </si>
-  <si>
-    <t>KT5</t>
-  </si>
-  <si>
     <t>Ngày</t>
   </si>
   <si>
@@ -132,6 +111,9 @@
   </si>
   <si>
     <t>Năm</t>
+  </si>
+  <si>
+    <t>DL1</t>
   </si>
 </sst>
 </file>
@@ -328,6 +310,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -351,12 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
@@ -662,56 +644,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="21" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="16"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="10">
-        <v>123</v>
-      </c>
-      <c r="I2" s="17" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="18"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="20"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="E3" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="4"/>
+      <c r="E3" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="11">
+        <v>2</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="4">
+        <v>2019</v>
+      </c>
     </row>
     <row r="4" spans="1:14" s="5" customFormat="1" ht="56.25">
       <c r="A4" s="4" t="s">
@@ -758,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2">
-        <v>9328</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -767,7 +755,7 @@
         <v>16198</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>16</v>
@@ -776,61 +764,20 @@
         <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" ht="37.5">
-      <c r="A6" s="2">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>9329</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="6">
-        <v>16198</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="D7" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>